<commit_message>
update project metadata extractor
</commit_message>
<xml_diff>
--- a/DBS/json_schema.xlsx
+++ b/DBS/json_schema.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DY\Desktop\Bio Data\BaseData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DY\Desktop\BioSampleManager\DBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF2CA7E-1673-4B95-9587-E7408BC10658}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C78C0D-879F-4408-AAE3-D1A90850EB96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
@@ -57,30 +57,15 @@
     <t>title</t>
   </si>
   <si>
-    <t>Publication title, if provided.</t>
-  </si>
-  <si>
     <t>topic</t>
   </si>
   <si>
     <t>Topic of given paper, select one or multiple from `aging`, `bioinformaticstool`, `brainorganoids`, `cancer`, `cardiology`, `cellbiology`, `developmentalbiology`, `disease`, `drugaddiction`, `epigenetics`, `fibrosis`, `hematopoiesis`, `host-viralinteractions`, `immunology`, `infectiousdisease`, `inflammation`, `metabolism`, `methodspaper`, `multi-omics`, `neuroscience`, `organtransplantation`, `pathogenesis`, `proteomics`, `psychiatricdisorders`, `pulmonology`, `regeneration`, `relhomeostasis`, `review`, `sensory`, `single-cellanalysis`, `stemcells`, `Tcellbiology`, `tissueengineering`, `transcriptomics`, or `Noneofabove`. Store as python list format.</t>
   </si>
   <si>
-    <t>project_title</t>
-  </si>
-  <si>
-    <t>Title of this project.</t>
-  </si>
-  <si>
     <t>Description or abstrcut of what this project studied.</t>
   </si>
   <si>
-    <t>is_cancer</t>
-  </si>
-  <si>
-    <t>Whether is this project research about cancer. `TRUE` or `FALSE`, `NS` if no hint.</t>
-  </si>
-  <si>
     <t>species</t>
   </si>
   <si>
@@ -93,30 +78,9 @@
     <t>Organisation(s) of sample sampling in the study, e.g. `boold`, `lung`. Store as python list format.</t>
   </si>
   <si>
-    <t>sample_location</t>
-  </si>
-  <si>
-    <t>Detailed sampling location, if given.</t>
-  </si>
-  <si>
     <t>library_strategy</t>
   </si>
   <si>
-    <t>Seqencing library strategy, if given. e.g. RNA-Seq</t>
-  </si>
-  <si>
-    <t>library_layout</t>
-  </si>
-  <si>
-    <t>select from `PAIRED` or `SINGLE`, and `NA` if not given.</t>
-  </si>
-  <si>
-    <t>single_cell</t>
-  </si>
-  <si>
-    <t>Whether it is single-cell level resolution, `TRUE`, `FALSE` or `NS` if no hint. e.g. scRNA-seq is `TRUE`</t>
-  </si>
-  <si>
     <t>nuclei_extraction</t>
   </si>
   <si>
@@ -124,21 +88,6 @@
   </si>
   <si>
     <t>technology_name</t>
-  </si>
-  <si>
-    <t>Name of single cell sequenceing technology used in project, e.g. SMART-seq2, or 10x 3' V3.</t>
-  </si>
-  <si>
-    <t>instrument</t>
-  </si>
-  <si>
-    <t>Sequencing instrucment.</t>
-  </si>
-  <si>
-    <t>Description of the extraction process for the target molecule in project.</t>
-  </si>
-  <si>
-    <t>Description of the data processing steps, including RAW data proccessing.</t>
   </si>
   <si>
     <t>Type</t>
@@ -148,22 +97,43 @@
     <t>list</t>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>Field</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>other_ids</t>
+  </si>
+  <si>
+    <t>INSDC or other project IDs, in python list format.</t>
+  </si>
+  <si>
+    <t>Project title, if provided.</t>
+  </si>
+  <si>
+    <t>resolution</t>
+  </si>
+  <si>
+    <t>The study resolution of this research, `Single-cell` for single-cell/single-nucleus research using technics such as 10x genomics 3' RNA-seq; `Spatial` for special omics tech such as 10x visum; `Bulk` for bulk level research; or `NS` if not speicific.</t>
+  </si>
+  <si>
+    <t>Name of single cell sequenceing technology used in project, e.g. `SMART-seq2`, `10x genomics chromium single cell 3'` (or `10x 3' V3` for short, depent on the authors description), or `NS` if not specific. In python list format. Please extract the author's original statements.</t>
+  </si>
+  <si>
+    <t>disease</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
     <t>project_description</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>extraction_protocol</t>
+    <t>What kind of disease involved in this research, in python list format, and use `Normal` for indicate non-diease samples were involved.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>data_processing</t>
+    <t>Seqencing library strategy, if given. e.g. `RNA-Seq`, `ATAC-Seq`, `DNA-Seq` etc, in python list format.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -499,23 +469,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="33" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -526,7 +499,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -537,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -548,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -559,183 +532,128 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>